<commit_message>
Y-axis on excel graph in (s)
</commit_message>
<xml_diff>
--- a/Assignment3/regression/results.xlsx
+++ b/Assignment3/regression/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\repos\MillerMill\Assignment3\regression_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\repos\MillerMill\Assignment3\regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -673,7 +673,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0036715281465693E-3"/>
+                  <c:y val="-1.5996702338897596E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1332,11 +1337,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="479383648"/>
-        <c:axId val="479376984"/>
+        <c:axId val="265870416"/>
+        <c:axId val="265870808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="479383648"/>
+        <c:axId val="265870416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1435,12 +1440,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479376984"/>
+        <c:crossAx val="265870808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="479376984"/>
+        <c:axId val="265870808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1481,7 +1486,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Processing Time</a:t>
+                  <a:t>Processing Time (s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1553,7 +1558,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479383648"/>
+        <c:crossAx val="265870416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2459,7 +2464,7 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>